<commit_message>
Add a ieee14 case for ConnMan debugging
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_conn.xlsx
+++ b/andes/cases/ieee14/ieee14_conn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFE50C4-E80B-A344-8E95-3A9A1AD20CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C3E821-C2A8-FF4F-B2D0-63736967F9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1700" windowWidth="27220" windowHeight="17000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="-20060" windowWidth="34560" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -624,7 +624,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -932,9 +932,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1607,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>162</v>
@@ -2310,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>

</xml_diff>